<commit_message>
0.0.6: use ktfmt for kotlin formatter. now blancoValueObjectKt should use more than 11 JDK.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8B7BA6-F00C-5C47-BABF-86119B78E067}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1F1CF5-130D-024F-9527-688D614D27A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -52,7 +52,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
   <si>
     <t>クラス名</t>
   </si>
@@ -300,18 +302,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>JsonProperty\\NotNull</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>JsonAutoDetect</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>NotNull</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>Nullable</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -398,6 +388,28 @@
   </si>
   <si>
     <t>abstract</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonProperty
+@NotNull</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@JsonAutoDetect(
+    "hoge: fuga")
+@NotNull</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@NotNull
+@JsonProperty(
+    "option: fuga"
+)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>NotNull</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1011,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1154,40 +1166,49 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1602,8 +1623,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1648,7 +1669,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="90"/>
+      <c r="G5" s="80"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
@@ -1664,7 +1685,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="91"/>
+      <c r="G6" s="81"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -1681,7 +1702,7 @@
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="91"/>
+      <c r="G7" s="81"/>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
@@ -1698,24 +1719,24 @@
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="91"/>
+      <c r="G8" s="81"/>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" ht="45">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
-        <v>51</v>
+      <c r="C9" s="84" t="s">
+        <v>68</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="91"/>
+      <c r="G9" s="81"/>
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
@@ -1726,13 +1747,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="92"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="82"/>
       <c r="H10" s="69"/>
       <c r="I10" s="69"/>
       <c r="J10" s="69"/>
@@ -1751,7 +1772,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="91"/>
+      <c r="G11" s="81"/>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
@@ -1776,14 +1797,14 @@
     </row>
     <row r="13" spans="1:13" s="33" customFormat="1">
       <c r="A13" s="66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" s="67"/>
       <c r="C13" s="68" t="s">
         <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -1795,7 +1816,7 @@
     </row>
     <row r="14" spans="1:13" s="33" customFormat="1">
       <c r="A14" s="66" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14" s="67"/>
       <c r="C14" s="68"/>
@@ -1810,7 +1831,7 @@
     </row>
     <row r="15" spans="1:13" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B15" s="67"/>
       <c r="C15" s="68" t="s">
@@ -1957,7 +1978,7 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" s="31" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -1979,7 +2000,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
@@ -2106,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C32" s="42"/>
       <c r="D32" s="42"/>
@@ -2190,57 +2211,57 @@
       <c r="O36" s="15"/>
     </row>
     <row r="37" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A37" s="84" t="s">
+      <c r="A37" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="83" t="s">
+      <c r="C37" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="83" t="s">
+      <c r="D37" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="85" t="s">
+      <c r="E37" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="83" t="s">
+      <c r="F37" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="H37" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="I37" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="J37" s="88" t="s">
-        <v>61</v>
-      </c>
-      <c r="K37" s="83" t="s">
+      <c r="G37" s="91" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="J37" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="83"/>
+      <c r="L37" s="89"/>
       <c r="M37" s="16"/>
       <c r="N37" s="17"/>
       <c r="O37" s="9"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="A38" s="84"/>
-      <c r="B38" s="84"/>
-      <c r="C38" s="83"/>
-      <c r="D38" s="83"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="83"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="83"/>
+      <c r="A38" s="90"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="92"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="93"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="95"/>
+      <c r="J38" s="95"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
       <c r="M38" s="18"/>
       <c r="N38" s="30"/>
       <c r="O38" s="15"/>
@@ -2250,14 +2271,14 @@
         <v>1</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F39" s="21" t="s">
         <v>34</v>
@@ -2278,20 +2299,20 @@
       <c r="N39" s="29"/>
       <c r="O39" s="15"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" ht="60">
       <c r="A40" s="19">
         <f>A39+1</f>
         <v>2</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D40" s="21"/>
-      <c r="E40" s="21" t="s">
-        <v>52</v>
+      <c r="E40" s="85" t="s">
+        <v>69</v>
       </c>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
@@ -2336,7 +2357,7 @@
       <c r="N41" s="23"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" ht="30">
       <c r="A42" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2348,8 +2369,8 @@
         <v>25</v>
       </c>
       <c r="D42" s="21"/>
-      <c r="E42" s="21" t="s">
-        <v>50</v>
+      <c r="E42" s="85" t="s">
+        <v>67</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
@@ -2364,7 +2385,7 @@
       <c r="N42" s="23"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" ht="15">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2376,8 +2397,8 @@
         <v>20</v>
       </c>
       <c r="D43" s="21"/>
-      <c r="E43" s="21" t="s">
-        <v>52</v>
+      <c r="E43" s="83" t="s">
+        <v>70</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -2425,7 +2446,7 @@
     <mergeCell ref="G37:G38"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
-  <dataValidations count="7">
+  <dataValidations disablePrompts="1" count="7">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F60:J60" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
@@ -2456,7 +2477,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D7EF1AF-B173-884C-9E34-724A844BDD2E}">
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
@@ -2524,10 +2545,10 @@
         <v>37</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F3" s="60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H3" s="60" t="s">
         <v>38</v>
@@ -2542,7 +2563,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="60" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -2551,7 +2572,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H4" s="62"/>
       <c r="J4" s="62"/>

</xml_diff>

<commit_message>
0.0.15: Enable kotlin specific class annotation, annotationKt.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1F1CF5-130D-024F-9527-688D614D27A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8422A9-7101-D646-AF0B-F3F259129B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>クラス名</t>
   </si>
@@ -410,6 +410,18 @@
   </si>
   <si>
     <t>NotNull</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>アノテーション(Kt)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>@Introspected</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>io.micronaut.core.annotation.Introspected</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1621,10 +1633,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1742,70 +1754,68 @@
       <c r="J9" s="38"/>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" spans="1:13" ht="29" customHeight="1">
+    <row r="10" spans="1:13" ht="15">
       <c r="A10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="84" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+    </row>
+    <row r="11" spans="1:13" ht="29" customHeight="1">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="86" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
     </row>
-    <row r="12" spans="1:13" s="33" customFormat="1">
-      <c r="A12" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="67"/>
-      <c r="C12" s="68"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="73"/>
-      <c r="K12"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
     </row>
     <row r="13" spans="1:13" s="33" customFormat="1">
       <c r="A13" s="66" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B13" s="67"/>
-      <c r="C13" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
-      </c>
+      <c r="C13" s="68"/>
+      <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -1816,11 +1826,15 @@
     </row>
     <row r="14" spans="1:13" s="33" customFormat="1">
       <c r="A14" s="66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-      <c r="D14"/>
+      <c r="C14" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -1831,12 +1845,10 @@
     </row>
     <row r="15" spans="1:13" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="67"/>
-      <c r="C15" s="68" t="s">
-        <v>45</v>
-      </c>
+      <c r="C15" s="68"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
@@ -1848,7 +1860,7 @@
     </row>
     <row r="16" spans="1:13" s="33" customFormat="1">
       <c r="A16" s="66" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B16" s="67"/>
       <c r="C16" s="68" t="s">
@@ -1865,7 +1877,7 @@
     </row>
     <row r="17" spans="1:15" s="33" customFormat="1">
       <c r="A17" s="66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="67"/>
       <c r="C17" s="68" t="s">
@@ -1880,83 +1892,85 @@
       <c r="J17" s="73"/>
       <c r="K17"/>
     </row>
-    <row r="18" spans="1:15" s="41" customFormat="1">
-      <c r="A18" s="38"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="31" t="s">
+    <row r="18" spans="1:15" s="33" customFormat="1">
+      <c r="A18" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="73"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:15" s="41" customFormat="1">
+      <c r="A19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
       <c r="L20" s="33"/>
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="39"/>
+      <c r="A21" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="77"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="76"/>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
@@ -1964,12 +1978,14 @@
       <c r="K22" s="39"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="38"/>
-      <c r="B23" s="40"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
+      <c r="A23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="77"/>
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
@@ -1977,69 +1993,65 @@
       <c r="K23" s="39"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="38"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39"/>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="51" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="46" t="s">
+      <c r="B26" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="48"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="39"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="55"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="40"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
       <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15">
       <c r="A27" s="55"/>
       <c r="B27" s="50"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="45"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
       <c r="I27" s="72"/>
@@ -2051,12 +2063,12 @@
       <c r="O27" s="39"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="56"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="54"/>
+      <c r="A28" s="55"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="72"/>
       <c r="H28" s="72"/>
       <c r="I28" s="72"/>
@@ -2067,89 +2079,89 @@
       <c r="N28" s="40"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" s="41" customFormat="1">
-      <c r="A29" s="38"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+    <row r="29" spans="1:15">
+      <c r="A29" s="56"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="38"/>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="31" t="s">
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="39"/>
+    </row>
+    <row r="30" spans="1:15" s="41" customFormat="1">
+      <c r="A30" s="38"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="51" t="s">
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="46" t="s">
+      <c r="B32" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="48"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="39"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="55">
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="39"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="55">
         <v>1</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B33" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="39"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="55"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="43"/>
       <c r="G33" s="72"/>
       <c r="H33" s="72"/>
       <c r="I33" s="72"/>
@@ -2161,12 +2173,16 @@
       <c r="O33" s="39"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="56"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="54"/>
+      <c r="A34" s="55">
+        <v>2</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="72"/>
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
@@ -2178,227 +2194,216 @@
       <c r="O34" s="39"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
+      <c r="A35" s="56"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="40"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="39"/>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="15"/>
-    </row>
-    <row r="37" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A37" s="90" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="15"/>
+    </row>
+    <row r="38" spans="1:15" ht="13.5" customHeight="1">
+      <c r="A38" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="90" t="s">
+      <c r="B38" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="89" t="s">
+      <c r="C38" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="89" t="s">
+      <c r="D38" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="91" t="s">
+      <c r="E38" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="89" t="s">
+      <c r="F38" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="91" t="s">
+      <c r="G38" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="H37" s="91" t="s">
+      <c r="H38" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="94" t="s">
+      <c r="I38" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="J37" s="94" t="s">
+      <c r="J38" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="K37" s="89" t="s">
+      <c r="K38" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="L37" s="89"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="17"/>
-      <c r="O37" s="9"/>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="90"/>
-      <c r="B38" s="90"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="89"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="93"/>
-      <c r="I38" s="95"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="89"/>
       <c r="L38" s="89"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="15"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="9"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="A39" s="19">
+      <c r="A39" s="90"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="89"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="95"/>
+      <c r="J39" s="95"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="30"/>
+      <c r="O39" s="15"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" s="19">
         <v>1</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B40" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C40" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21" t="s">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G39" s="21"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="J39" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="29"/>
-      <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="1:15" ht="60">
-      <c r="A40" s="19">
-        <f>A39+1</f>
-        <v>2</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D40" s="21"/>
-      <c r="E40" s="85" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
+      <c r="I40" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="J40" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="21"/>
+      <c r="K40" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="29"/>
       <c r="O40" s="15"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" ht="60">
       <c r="A41" s="19">
-        <f t="shared" ref="A41:A43" si="0">A40+1</f>
-        <v>3</v>
+        <f>A40+1</f>
+        <v>2</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="21"/>
+        <v>54</v>
+      </c>
+      <c r="D41" s="21"/>
+      <c r="E41" s="85" t="s">
+        <v>69</v>
+      </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="78" t="s">
+      <c r="H41" s="78"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="21" t="s">
-        <v>18</v>
-      </c>
+      <c r="K41" s="21"/>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
-      <c r="N41" s="23"/>
+      <c r="N41" s="29"/>
       <c r="O41" s="15"/>
     </row>
-    <row r="42" spans="1:15" ht="30">
+    <row r="42" spans="1:15">
       <c r="A42" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A42:A44" si="0">A41+1</f>
+        <v>3</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D42" s="21"/>
-      <c r="E42" s="85" t="s">
-        <v>67</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="21"/>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
-      <c r="H42" s="78"/>
+      <c r="H42" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="I42" s="78"/>
       <c r="J42" s="78"/>
       <c r="K42" s="21" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="23"/>
       <c r="O42" s="15"/>
     </row>
-    <row r="43" spans="1:15" ht="15">
+    <row r="43" spans="1:15" ht="30">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D43" s="21"/>
-      <c r="E43" s="83" t="s">
-        <v>70</v>
+      <c r="E43" s="85" t="s">
+        <v>67</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -2406,67 +2411,95 @@
       <c r="I43" s="78"/>
       <c r="J43" s="78"/>
       <c r="K43" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="23"/>
       <c r="O43" s="15"/>
     </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="79"/>
-      <c r="I44" s="79"/>
-      <c r="J44" s="79"/>
-      <c r="K44" s="26"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="28"/>
+    <row r="44" spans="1:15" ht="15">
+      <c r="A44" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="78"/>
+      <c r="J44" s="78"/>
+      <c r="K44" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="23"/>
       <c r="O44" s="15"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="K37:L38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="G38:G39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations disablePrompts="1" count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F60:J60" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:J61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 G39:G44" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 G40:G45" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
       <formula1>isFinal</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
       <formula1>isData</formula1>
     </dataValidation>
   </dataValidations>
@@ -2482,7 +2515,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H39:J44</xm:sqref>
+          <xm:sqref>H40:J45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
0.0.16: Not output unnecessary public keyword.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8422A9-7101-D646-AF0B-F3F259129B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607055D-7E94-BA48-BB1F-BA348AA74CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
   <si>
     <t>クラス名</t>
   </si>
@@ -423,6 +423,9 @@
   <si>
     <t>io.micronaut.core.annotation.Introspected</t>
     <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1639,7 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1814,7 +1817,9 @@
         <v>37</v>
       </c>
       <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
+      <c r="C13" s="68" t="s">
+        <v>74</v>
+      </c>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -2479,7 +2484,7 @@
     <mergeCell ref="G38:G39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
-  <dataValidations disablePrompts="1" count="7">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:J61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
@@ -2510,7 +2515,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D7EF1AF-B173-884C-9E34-724A844BDD2E}">
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>

</xml_diff>

<commit_message>
0.0.19: Extends and Implements packages are preferred with pre-generated objects packages, if found.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A607055D-7E94-BA48-BB1F-BA348AA74CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E909EA-0295-244D-B2F8-9E5353C41281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
   <si>
     <t>クラス名</t>
   </si>
@@ -426,6 +426,14 @@
   </si>
   <si>
     <t>public</t>
+  </si>
+  <si>
+    <t>SimpleSample2</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>java.lang.Throwable</t>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
@@ -1638,8 +1646,8 @@
   </sheetPr>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1953,7 +1961,9 @@
         <v>0</v>
       </c>
       <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="36" t="s">
+        <v>75</v>
+      </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
       <c r="F21" s="75"/>
@@ -1972,7 +1982,9 @@
         <v>22</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
       <c r="F22" s="76"/>
@@ -2051,8 +2063,12 @@
       <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="55"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="55">
+        <v>1</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>76</v>
+      </c>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
       <c r="E27" s="42"/>

</xml_diff>

<commit_message>
0.0.21: Required field is added to field list, that is converted to @NotNull annotaion.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E909EA-0295-244D-B2F8-9E5353C41281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BCD1E5-3413-044D-82BB-2F301C1E850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
   <si>
     <t>クラス名</t>
   </si>
@@ -433,6 +433,13 @@
   </si>
   <si>
     <t>java.lang.Throwable</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>必須</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヒッス </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1644,10 +1651,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1656,34 +1663,34 @@
     <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28" style="1" customWidth="1"/>
-    <col min="14" max="14" width="33.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="9" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="1" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19">
+    <row r="1" spans="1:14" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1696,8 +1703,9 @@
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1712,9 +1720,10 @@
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="38"/>
+      <c r="L6" s="39"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1729,9 +1738,10 @@
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1746,9 +1756,10 @@
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
-      <c r="K8" s="39"/>
-    </row>
-    <row r="9" spans="1:13" ht="45">
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="1:14" ht="45">
       <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1763,9 +1774,10 @@
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
-      <c r="K9" s="39"/>
-    </row>
-    <row r="10" spans="1:13" ht="15">
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+    </row>
+    <row r="10" spans="1:14" ht="15">
       <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
@@ -1780,9 +1792,10 @@
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:13" ht="29" customHeight="1">
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:14" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1797,11 +1810,12 @@
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
-      <c r="K11" s="38"/>
+      <c r="K11" s="69"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="38"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1819,8 +1833,9 @@
       <c r="K12" s="38"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
-    </row>
-    <row r="13" spans="1:13" s="33" customFormat="1">
+      <c r="N12" s="38"/>
+    </row>
+    <row r="13" spans="1:14" s="33" customFormat="1">
       <c r="A13" s="66" t="s">
         <v>37</v>
       </c>
@@ -1834,10 +1849,11 @@
       <c r="G13"/>
       <c r="H13" s="70"/>
       <c r="I13" s="70"/>
-      <c r="J13" s="73"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:13" s="33" customFormat="1">
+      <c r="J13" s="70"/>
+      <c r="K13" s="73"/>
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:14" s="33" customFormat="1">
       <c r="A14" s="66" t="s">
         <v>63</v>
       </c>
@@ -1853,10 +1869,11 @@
       <c r="G14"/>
       <c r="H14" s="70"/>
       <c r="I14" s="70"/>
-      <c r="J14" s="73"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:13" s="33" customFormat="1">
+      <c r="J14" s="70"/>
+      <c r="K14" s="73"/>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:14" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
         <v>61</v>
       </c>
@@ -1868,10 +1885,11 @@
       <c r="G15"/>
       <c r="H15" s="70"/>
       <c r="I15" s="70"/>
-      <c r="J15" s="73"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:13" s="33" customFormat="1">
+      <c r="J15" s="70"/>
+      <c r="K15" s="73"/>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:14" s="33" customFormat="1">
       <c r="A16" s="66" t="s">
         <v>62</v>
       </c>
@@ -1885,10 +1903,11 @@
       <c r="G16"/>
       <c r="H16" s="70"/>
       <c r="I16" s="70"/>
-      <c r="J16" s="73"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:15" s="33" customFormat="1">
+      <c r="J16" s="70"/>
+      <c r="K16" s="73"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:16" s="33" customFormat="1">
       <c r="A17" s="66" t="s">
         <v>44</v>
       </c>
@@ -1902,10 +1921,11 @@
       <c r="G17"/>
       <c r="H17" s="70"/>
       <c r="I17" s="70"/>
-      <c r="J17" s="73"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:15" s="33" customFormat="1">
+      <c r="J17" s="70"/>
+      <c r="K17" s="73"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:16" s="33" customFormat="1">
       <c r="A18" s="66" t="s">
         <v>46</v>
       </c>
@@ -1919,10 +1939,11 @@
       <c r="G18"/>
       <c r="H18" s="70"/>
       <c r="I18" s="70"/>
-      <c r="J18" s="73"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:15" s="41" customFormat="1">
+      <c r="J18" s="70"/>
+      <c r="K18" s="73"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:16" s="41" customFormat="1">
       <c r="A19" s="38"/>
       <c r="B19" s="40"/>
       <c r="C19" s="38"/>
@@ -1936,8 +1957,9 @@
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="N19" s="38"/>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="31" t="s">
         <v>16</v>
       </c>
@@ -1951,12 +1973,13 @@
       <c r="I20" s="48"/>
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
-      <c r="L20" s="33"/>
+      <c r="L20" s="48"/>
       <c r="M20" s="33"/>
       <c r="N20" s="33"/>
       <c r="O20" s="33"/>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" s="33"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="34" t="s">
         <v>0</v>
       </c>
@@ -1972,12 +1995,13 @@
       <c r="I21" s="71"/>
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
-      <c r="L21" s="33"/>
+      <c r="L21" s="71"/>
       <c r="M21" s="33"/>
       <c r="N21" s="33"/>
       <c r="O21" s="33"/>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1992,9 +2016,10 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
-      <c r="K22" s="39"/>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="K22" s="38"/>
+      <c r="L22" s="39"/>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -2007,9 +2032,10 @@
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
-      <c r="K23" s="39"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="38"/>
       <c r="B24" s="40"/>
       <c r="C24" s="38"/>
@@ -2020,9 +2046,10 @@
       <c r="H24" s="38"/>
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="K24" s="38"/>
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="31" t="s">
         <v>56</v>
       </c>
@@ -2036,12 +2063,13 @@
       <c r="I25" s="48"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
-      <c r="L25" s="47"/>
+      <c r="L25" s="48"/>
       <c r="M25" s="47"/>
       <c r="N25" s="47"/>
       <c r="O25" s="47"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="47"/>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="51" t="s">
         <v>32</v>
       </c>
@@ -2057,12 +2085,13 @@
       <c r="I26" s="71"/>
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="49"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="48"/>
       <c r="N26" s="49"/>
-      <c r="O26" s="39"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="O26" s="49"/>
+      <c r="P26" s="39"/>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="55">
         <v>1</v>
       </c>
@@ -2077,13 +2106,14 @@
       <c r="H27" s="72"/>
       <c r="I27" s="72"/>
       <c r="J27" s="72"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="40"/>
+      <c r="K27" s="72"/>
+      <c r="L27" s="38"/>
       <c r="M27" s="40"/>
       <c r="N27" s="40"/>
-      <c r="O27" s="39"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="O27" s="40"/>
+      <c r="P27" s="39"/>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="55"/>
       <c r="B28" s="50"/>
       <c r="C28" s="44"/>
@@ -2094,13 +2124,14 @@
       <c r="H28" s="72"/>
       <c r="I28" s="72"/>
       <c r="J28" s="72"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="40"/>
+      <c r="K28" s="72"/>
+      <c r="L28" s="38"/>
       <c r="M28" s="40"/>
       <c r="N28" s="40"/>
-      <c r="O28" s="39"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="O28" s="40"/>
+      <c r="P28" s="39"/>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="56"/>
       <c r="B29" s="52"/>
       <c r="C29" s="53"/>
@@ -2111,13 +2142,14 @@
       <c r="H29" s="72"/>
       <c r="I29" s="72"/>
       <c r="J29" s="72"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="40"/>
+      <c r="K29" s="72"/>
+      <c r="L29" s="38"/>
       <c r="M29" s="40"/>
       <c r="N29" s="40"/>
-      <c r="O29" s="39"/>
-    </row>
-    <row r="30" spans="1:15" s="41" customFormat="1">
+      <c r="O29" s="40"/>
+      <c r="P29" s="39"/>
+    </row>
+    <row r="30" spans="1:16" s="41" customFormat="1">
       <c r="A30" s="38"/>
       <c r="B30" s="40"/>
       <c r="C30" s="38"/>
@@ -2131,8 +2163,9 @@
       <c r="K30" s="38"/>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="N30" s="38"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="31" t="s">
         <v>31</v>
       </c>
@@ -2146,12 +2179,13 @@
       <c r="I31" s="48"/>
       <c r="J31" s="48"/>
       <c r="K31" s="48"/>
-      <c r="L31" s="47"/>
+      <c r="L31" s="48"/>
       <c r="M31" s="47"/>
       <c r="N31" s="47"/>
       <c r="O31" s="47"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" s="47"/>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="51" t="s">
         <v>32</v>
       </c>
@@ -2167,12 +2201,13 @@
       <c r="I32" s="71"/>
       <c r="J32" s="71"/>
       <c r="K32" s="71"/>
-      <c r="L32" s="48"/>
-      <c r="M32" s="49"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="48"/>
       <c r="N32" s="49"/>
-      <c r="O32" s="39"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="O32" s="49"/>
+      <c r="P32" s="39"/>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="55">
         <v>1</v>
       </c>
@@ -2187,13 +2222,14 @@
       <c r="H33" s="72"/>
       <c r="I33" s="72"/>
       <c r="J33" s="72"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="40"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="38"/>
       <c r="M33" s="40"/>
       <c r="N33" s="40"/>
-      <c r="O33" s="39"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="O33" s="40"/>
+      <c r="P33" s="39"/>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="55">
         <v>2</v>
       </c>
@@ -2208,13 +2244,14 @@
       <c r="H34" s="72"/>
       <c r="I34" s="72"/>
       <c r="J34" s="72"/>
-      <c r="K34" s="38"/>
-      <c r="L34" s="40"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="38"/>
       <c r="M34" s="40"/>
       <c r="N34" s="40"/>
-      <c r="O34" s="39"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="O34" s="40"/>
+      <c r="P34" s="39"/>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="56"/>
       <c r="B35" s="52"/>
       <c r="C35" s="53"/>
@@ -2225,13 +2262,14 @@
       <c r="H35" s="72"/>
       <c r="I35" s="72"/>
       <c r="J35" s="72"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="40"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="38"/>
       <c r="M35" s="40"/>
       <c r="N35" s="40"/>
-      <c r="O35" s="39"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="O35" s="40"/>
+      <c r="P35" s="39"/>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2244,8 +2282,9 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="M36" s="13"/>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
@@ -2261,10 +2300,11 @@
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="15"/>
-    </row>
-    <row r="38" spans="1:15" ht="13.5" customHeight="1">
+      <c r="N37" s="14"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="15"/>
+    </row>
+    <row r="38" spans="1:16" ht="13.5" customHeight="1">
       <c r="A38" s="90" t="s">
         <v>32</v>
       </c>
@@ -2290,20 +2330,23 @@
         <v>50</v>
       </c>
       <c r="I38" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="J38" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="J38" s="94" t="s">
+      <c r="K38" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="K38" s="89" t="s">
+      <c r="L38" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="L38" s="89"/>
-      <c r="M38" s="16"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="9"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="M38" s="89"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="9"/>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="90"/>
       <c r="B39" s="90"/>
       <c r="C39" s="89"/>
@@ -2314,13 +2357,14 @@
       <c r="H39" s="93"/>
       <c r="I39" s="95"/>
       <c r="J39" s="95"/>
-      <c r="K39" s="89"/>
+      <c r="K39" s="95"/>
       <c r="L39" s="89"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="15"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="M39" s="89"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="30"/>
+      <c r="P39" s="15"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="19">
         <v>1</v>
       </c>
@@ -2338,22 +2382,27 @@
         <v>34</v>
       </c>
       <c r="G40" s="21"/>
-      <c r="H40" s="78"/>
+      <c r="H40" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="I40" s="78" t="s">
         <v>45</v>
       </c>
       <c r="J40" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="21" t="s">
+      <c r="K40" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="L40" s="22"/>
       <c r="M40" s="22"/>
-      <c r="N40" s="29"/>
-      <c r="O40" s="15"/>
-    </row>
-    <row r="41" spans="1:15" ht="60">
+      <c r="N40" s="22"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="15"/>
+    </row>
+    <row r="41" spans="1:16" ht="60">
       <c r="A41" s="19">
         <f>A40+1</f>
         <v>2</v>
@@ -2372,16 +2421,17 @@
       <c r="G41" s="21"/>
       <c r="H41" s="78"/>
       <c r="I41" s="78"/>
-      <c r="J41" s="78" t="s">
+      <c r="J41" s="78"/>
+      <c r="K41" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="K41" s="21"/>
-      <c r="L41" s="22"/>
+      <c r="L41" s="21"/>
       <c r="M41" s="22"/>
-      <c r="N41" s="29"/>
-      <c r="O41" s="15"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="N41" s="22"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="15"/>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="19">
         <f t="shared" ref="A42:A44" si="0">A41+1</f>
         <v>3</v>
@@ -2403,15 +2453,16 @@
       </c>
       <c r="I42" s="78"/>
       <c r="J42" s="78"/>
-      <c r="K42" s="21" t="s">
+      <c r="K42" s="78"/>
+      <c r="L42" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="22"/>
       <c r="M42" s="22"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="15"/>
-    </row>
-    <row r="43" spans="1:15" ht="30">
+      <c r="N42" s="22"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="15"/>
+    </row>
+    <row r="43" spans="1:16" ht="30">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2431,15 +2482,16 @@
       <c r="H43" s="78"/>
       <c r="I43" s="78"/>
       <c r="J43" s="78"/>
-      <c r="K43" s="21" t="s">
+      <c r="K43" s="78"/>
+      <c r="L43" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="L43" s="22"/>
       <c r="M43" s="22"/>
-      <c r="N43" s="23"/>
-      <c r="O43" s="15"/>
-    </row>
-    <row r="44" spans="1:15" ht="15">
+      <c r="N43" s="22"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="15"/>
+    </row>
+    <row r="44" spans="1:16" ht="15">
       <c r="A44" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2459,15 +2511,16 @@
       <c r="H44" s="78"/>
       <c r="I44" s="78"/>
       <c r="J44" s="78"/>
-      <c r="K44" s="21" t="s">
+      <c r="K44" s="78"/>
+      <c r="L44" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L44" s="22"/>
       <c r="M44" s="22"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="15"/>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="N44" s="22"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="15"/>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" s="24"/>
       <c r="B45" s="25"/>
       <c r="C45" s="26"/>
@@ -2478,16 +2531,17 @@
       <c r="H45" s="79"/>
       <c r="I45" s="79"/>
       <c r="J45" s="79"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="27"/>
+      <c r="K45" s="79"/>
+      <c r="L45" s="26"/>
       <c r="M45" s="27"/>
-      <c r="N45" s="28"/>
-      <c r="O45" s="15"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="L38:M39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
@@ -2495,13 +2549,14 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="H38:H39"/>
+    <mergeCell ref="K38:K39"/>
     <mergeCell ref="J38:J39"/>
+    <mergeCell ref="G38:G39"/>
     <mergeCell ref="I38:I39"/>
-    <mergeCell ref="G38:G39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:J61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:K61" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2536,7 +2591,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H40:J45</xm:sqref>
+          <xm:sqref>H40:K45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
0.1.2: Enable requiredKt, NullableKt, fixedValueKt columns for fieldList.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BCD1E5-3413-044D-82BB-2F301C1E850E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557774BA-60CE-F34C-9DF8-B6D4C6C393FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,7 @@
     <definedName name="Submit有無" localSheetId="1">#REF!</definedName>
     <definedName name="Submit有無">#REF!</definedName>
     <definedName name="theOther">config!$P$4:$P$5</definedName>
+    <definedName name="threeAlters">config!$R$4:$R$6</definedName>
     <definedName name="toString">config!$J$4:$J$5</definedName>
     <definedName name="Validate実装パターン" localSheetId="1">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
   <si>
     <t>クラス名</t>
   </si>
@@ -124,9 +125,6 @@
   <si>
     <t>array</t>
     <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>バリューオブジェクト定義(php)・継承</t>
   </si>
   <si>
     <t>arrayObject</t>
@@ -437,6 +435,45 @@
   </si>
   <si>
     <t>必須</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ヒッス </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>バリューオブジェクト定義(php)・継承</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>Nullable(Kt)</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>変更不可変数(Kt)</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">ヘンコウフカ </t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ヘンスウ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>×</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>三択</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">サンタク </t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>必須(Kt)</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">ヒッス </t>
     </rPh>
@@ -1053,7 +1090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1239,6 +1276,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1651,10 +1691,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1663,34 +1703,35 @@
     <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="28" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="28" style="1" customWidth="1"/>
+    <col min="18" max="18" width="33.33203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19">
+    <row r="1" spans="1:17" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1704,14 +1745,17 @@
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -1721,15 +1765,18 @@
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
-      <c r="L6" s="39"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="39"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -1739,15 +1786,18 @@
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
       <c r="K7" s="38"/>
-      <c r="L7" s="39"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="39"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -1757,15 +1807,18 @@
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
-      <c r="L8" s="39"/>
-    </row>
-    <row r="9" spans="1:14" ht="45">
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="39"/>
+    </row>
+    <row r="9" spans="1:17" ht="45">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="84" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -1775,15 +1828,18 @@
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
-      <c r="L9" s="39"/>
-    </row>
-    <row r="10" spans="1:14" ht="15">
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="39"/>
+    </row>
+    <row r="10" spans="1:17" ht="15">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
@@ -1793,15 +1849,18 @@
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
       <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
-    </row>
-    <row r="11" spans="1:14" ht="29" customHeight="1">
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="39"/>
+    </row>
+    <row r="11" spans="1:17" ht="29" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="86" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="87"/>
       <c r="E11" s="87"/>
@@ -1811,11 +1870,14 @@
       <c r="I11" s="69"/>
       <c r="J11" s="69"/>
       <c r="K11" s="69"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1834,14 +1896,17 @@
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
-    </row>
-    <row r="13" spans="1:14" s="33" customFormat="1">
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+    </row>
+    <row r="13" spans="1:17" s="33" customFormat="1">
       <c r="A13" s="66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="67"/>
       <c r="C13" s="68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -1850,19 +1915,22 @@
       <c r="H13" s="70"/>
       <c r="I13" s="70"/>
       <c r="J13" s="70"/>
-      <c r="K13" s="73"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:14" s="33" customFormat="1">
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="73"/>
+      <c r="O13"/>
+    </row>
+    <row r="14" spans="1:17" s="33" customFormat="1">
       <c r="A14" s="66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="67"/>
       <c r="C14" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -1870,12 +1938,15 @@
       <c r="H14" s="70"/>
       <c r="I14" s="70"/>
       <c r="J14" s="70"/>
-      <c r="K14" s="73"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:14" s="33" customFormat="1">
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
+      <c r="N14" s="73"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:17" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="67"/>
       <c r="C15" s="68"/>
@@ -1886,16 +1957,19 @@
       <c r="H15" s="70"/>
       <c r="I15" s="70"/>
       <c r="J15" s="70"/>
-      <c r="K15" s="73"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:14" s="33" customFormat="1">
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="73"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:17" s="33" customFormat="1">
       <c r="A16" s="66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="67"/>
       <c r="C16" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -1904,16 +1978,19 @@
       <c r="H16" s="70"/>
       <c r="I16" s="70"/>
       <c r="J16" s="70"/>
-      <c r="K16" s="73"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:16" s="33" customFormat="1">
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="73"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:19" s="33" customFormat="1">
       <c r="A17" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="67"/>
       <c r="C17" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -1922,16 +1999,19 @@
       <c r="H17" s="70"/>
       <c r="I17" s="70"/>
       <c r="J17" s="70"/>
-      <c r="K17" s="73"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:16" s="33" customFormat="1">
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="73"/>
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:19" s="33" customFormat="1">
       <c r="A18" s="66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="67"/>
       <c r="C18" s="68" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -1940,10 +2020,13 @@
       <c r="H18" s="70"/>
       <c r="I18" s="70"/>
       <c r="J18" s="70"/>
-      <c r="K18" s="73"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:16" s="41" customFormat="1">
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="73"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:19" s="41" customFormat="1">
       <c r="A19" s="38"/>
       <c r="B19" s="40"/>
       <c r="C19" s="38"/>
@@ -1958,10 +2041,13 @@
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
       <c r="N19" s="38"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="31" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
@@ -1974,18 +2060,21 @@
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
       <c r="L20" s="48"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
       <c r="P20" s="33"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
@@ -1996,18 +2085,21 @@
       <c r="J21" s="71"/>
       <c r="K21" s="71"/>
       <c r="L21" s="71"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
       <c r="P21" s="33"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="33"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
@@ -2017,11 +2109,14 @@
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
       <c r="K22" s="38"/>
-      <c r="L22" s="39"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -2033,9 +2128,12 @@
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
       <c r="K23" s="38"/>
-      <c r="L23" s="39"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="39"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="38"/>
       <c r="B24" s="40"/>
       <c r="C24" s="38"/>
@@ -2047,11 +2145,14 @@
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
       <c r="K24" s="38"/>
-      <c r="L24" s="39"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -2064,17 +2165,20 @@
       <c r="J25" s="48"/>
       <c r="K25" s="48"/>
       <c r="L25" s="48"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
-      <c r="O25" s="47"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
       <c r="P25" s="47"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="47"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="46"/>
       <c r="D26" s="46"/>
@@ -2086,17 +2190,20 @@
       <c r="J26" s="71"/>
       <c r="K26" s="71"/>
       <c r="L26" s="71"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="39"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="M26" s="71"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="48"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="39"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="55">
         <v>1</v>
       </c>
       <c r="B27" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="42"/>
@@ -2107,13 +2214,16 @@
       <c r="I27" s="72"/>
       <c r="J27" s="72"/>
       <c r="K27" s="72"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="39"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="L27" s="72"/>
+      <c r="M27" s="72"/>
+      <c r="N27" s="72"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="39"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="55"/>
       <c r="B28" s="50"/>
       <c r="C28" s="44"/>
@@ -2125,13 +2235,16 @@
       <c r="I28" s="72"/>
       <c r="J28" s="72"/>
       <c r="K28" s="72"/>
-      <c r="L28" s="38"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="39"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="L28" s="72"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="72"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="39"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="56"/>
       <c r="B29" s="52"/>
       <c r="C29" s="53"/>
@@ -2143,13 +2256,16 @@
       <c r="I29" s="72"/>
       <c r="J29" s="72"/>
       <c r="K29" s="72"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="39"/>
-    </row>
-    <row r="30" spans="1:16" s="41" customFormat="1">
+      <c r="L29" s="72"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="72"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="39"/>
+    </row>
+    <row r="30" spans="1:19" s="41" customFormat="1">
       <c r="A30" s="38"/>
       <c r="B30" s="40"/>
       <c r="C30" s="38"/>
@@ -2164,10 +2280,13 @@
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
       <c r="N30" s="38"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
@@ -2180,17 +2299,20 @@
       <c r="J31" s="48"/>
       <c r="K31" s="48"/>
       <c r="L31" s="48"/>
-      <c r="M31" s="47"/>
-      <c r="N31" s="47"/>
-      <c r="O31" s="47"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
       <c r="P31" s="47"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="46" t="s">
         <v>32</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>33</v>
       </c>
       <c r="C32" s="46"/>
       <c r="D32" s="46"/>
@@ -2202,17 +2324,20 @@
       <c r="J32" s="71"/>
       <c r="K32" s="71"/>
       <c r="L32" s="71"/>
-      <c r="M32" s="48"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="39"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="48"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="39"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="55">
         <v>1</v>
       </c>
       <c r="B33" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="42"/>
@@ -2223,18 +2348,21 @@
       <c r="I33" s="72"/>
       <c r="J33" s="72"/>
       <c r="K33" s="72"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="40"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="40"/>
-      <c r="P33" s="39"/>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="39"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="55">
         <v>2</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="44"/>
@@ -2245,13 +2373,16 @@
       <c r="I34" s="72"/>
       <c r="J34" s="72"/>
       <c r="K34" s="72"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="39"/>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="39"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="56"/>
       <c r="B35" s="52"/>
       <c r="C35" s="53"/>
@@ -2263,13 +2394,16 @@
       <c r="I35" s="72"/>
       <c r="J35" s="72"/>
       <c r="K35" s="72"/>
-      <c r="L35" s="38"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="40"/>
-      <c r="P35" s="39"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="40"/>
+      <c r="Q35" s="40"/>
+      <c r="R35" s="40"/>
+      <c r="S35" s="39"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -2283,8 +2417,11 @@
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="3" t="s">
         <v>11</v>
       </c>
@@ -2301,12 +2438,15 @@
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="15"/>
-    </row>
-    <row r="38" spans="1:16" ht="13.5" customHeight="1">
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="15"/>
+    </row>
+    <row r="38" spans="1:19" ht="13.5" customHeight="1">
       <c r="A38" s="90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="90" t="s">
         <v>4</v>
@@ -2315,38 +2455,47 @@
         <v>5</v>
       </c>
       <c r="D38" s="89" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E38" s="91" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F38" s="89" t="s">
         <v>6</v>
       </c>
       <c r="G38" s="91" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H38" s="91" t="s">
-        <v>50</v>
-      </c>
-      <c r="I38" s="94" t="s">
-        <v>77</v>
+        <v>49</v>
+      </c>
+      <c r="I38" s="91" t="s">
+        <v>78</v>
       </c>
       <c r="J38" s="94" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="K38" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="L38" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="L38" s="89" t="s">
+      <c r="M38" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="N38" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="O38" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="M38" s="89"/>
-      <c r="N38" s="16"/>
-      <c r="O38" s="17"/>
-      <c r="P38" s="9"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="P38" s="89"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="9"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="90"/>
       <c r="B39" s="90"/>
       <c r="C39" s="89"/>
@@ -2355,172 +2504,220 @@
       <c r="F39" s="89"/>
       <c r="G39" s="93"/>
       <c r="H39" s="93"/>
-      <c r="I39" s="95"/>
+      <c r="I39" s="93"/>
       <c r="J39" s="95"/>
       <c r="K39" s="95"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="15"/>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="L39" s="95"/>
+      <c r="M39" s="95"/>
+      <c r="N39" s="95"/>
+      <c r="O39" s="89"/>
+      <c r="P39" s="89"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="30"/>
+      <c r="S39" s="15"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="19">
         <v>1</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G40" s="21"/>
       <c r="H40" s="78" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I40" s="78" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J40" s="78" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K40" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="L40" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L40" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="M40" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="N40" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="O40" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="29"/>
-      <c r="P40" s="15"/>
-    </row>
-    <row r="41" spans="1:16" ht="60">
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="15"/>
+    </row>
+    <row r="41" spans="1:19" ht="60">
       <c r="A41" s="19">
         <f>A40+1</f>
         <v>2</v>
       </c>
       <c r="B41" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
-      <c r="H41" s="78"/>
+      <c r="H41" s="78" t="s">
+        <v>44</v>
+      </c>
       <c r="I41" s="78"/>
-      <c r="J41" s="78"/>
-      <c r="K41" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="L41" s="21"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-      <c r="O41" s="29"/>
-      <c r="P41" s="15"/>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="J41" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="78"/>
+      <c r="L41" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="M41" s="78"/>
+      <c r="N41" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="O41" s="21"/>
+      <c r="P41" s="22"/>
+      <c r="Q41" s="22"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="15"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="19">
         <f t="shared" ref="A42:A44" si="0">A41+1</f>
         <v>3</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E42" s="21"/>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
       <c r="H42" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="15"/>
-    </row>
-    <row r="43" spans="1:16" ht="30">
+        <v>44</v>
+      </c>
+      <c r="I42" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="J42" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="K42" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="L42" s="78"/>
+      <c r="M42" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="N42" s="78"/>
+      <c r="O42" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="15"/>
+    </row>
+    <row r="43" spans="1:19" ht="30">
       <c r="A43" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D43" s="21"/>
       <c r="E43" s="85" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
       <c r="H43" s="78"/>
-      <c r="I43" s="78"/>
+      <c r="I43" s="78" t="s">
+        <v>44</v>
+      </c>
       <c r="J43" s="78"/>
-      <c r="K43" s="78"/>
-      <c r="L43" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-      <c r="O43" s="23"/>
-      <c r="P43" s="15"/>
-    </row>
-    <row r="44" spans="1:16" ht="15">
+      <c r="K43" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="L43" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="M43" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="N43" s="78"/>
+      <c r="O43" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="P43" s="22"/>
+      <c r="Q43" s="22"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="15"/>
+    </row>
+    <row r="44" spans="1:19" ht="15">
       <c r="A44" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="21"/>
       <c r="E44" s="83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F44" s="21"/>
       <c r="G44" s="21"/>
       <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
+      <c r="I44" s="78" t="s">
+        <v>80</v>
+      </c>
       <c r="J44" s="78"/>
       <c r="K44" s="78"/>
-      <c r="L44" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="15"/>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="L44" s="78"/>
+      <c r="M44" s="78"/>
+      <c r="N44" s="78"/>
+      <c r="O44" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="15"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="24"/>
       <c r="B45" s="25"/>
       <c r="C45" s="26"/>
@@ -2532,34 +2729,36 @@
       <c r="I45" s="79"/>
       <c r="J45" s="79"/>
       <c r="K45" s="79"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="15"/>
+      <c r="L45" s="79"/>
+      <c r="M45" s="79"/>
+      <c r="N45" s="79"/>
+      <c r="O45" s="26"/>
+      <c r="P45" s="27"/>
+      <c r="Q45" s="27"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="K38:K39"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="L38:M39"/>
+    <mergeCell ref="O38:P39"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="J38:J39"/>
     <mergeCell ref="H38:H39"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="I38:I39"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:K61" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>型</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
@@ -2578,6 +2777,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
       <formula1>isData</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M40:M45 I40:I45 K40:K45" xr:uid="{AA44E717-1078-2342-AD63-3C06BBA1FD3D}">
+      <formula1>threeAlters</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F61:N61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>型</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.59027777777777779" right="0.59027777777777779" top="0.59027777777777779" bottom="0.59027777777777779" header="0.51180555555555562" footer="0.11805555555555557"/>
   <pageSetup paperSize="9" scale="82" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -2591,7 +2797,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H40:K45</xm:sqref>
+          <xm:sqref>N40:N45 H40:H45 J40:J45 L40:L45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2604,10 +2810,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="R4" sqref="R4:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -2628,9 +2834,9 @@
     <col min="261" max="16384" width="10.83203125" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="19">
+    <row r="1" spans="1:18" ht="19">
       <c r="A1" s="57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="57"/>
       <c r="C1" s="57"/>
@@ -2645,74 +2851,85 @@
       <c r="L1" s="57"/>
       <c r="M1" s="57"/>
       <c r="N1" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="58"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="B3" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="58"/>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="B3" s="60" t="s">
+      <c r="D3" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="60" t="s">
+      <c r="J3" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="60" t="s">
+      <c r="L3" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="N3" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="60" t="s">
-        <v>41</v>
-      </c>
       <c r="P3" s="60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>50</v>
+      </c>
+      <c r="R3" s="60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="B4" s="61"/>
       <c r="D4" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H4" s="62"/>
       <c r="J4" s="62"/>
       <c r="L4" s="62"/>
       <c r="N4" s="62"/>
       <c r="P4" s="62"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="62"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="B5" s="63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="64"/>
       <c r="F5" s="64"/>
       <c r="H5" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N5" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P5" s="64" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>42</v>
+      </c>
+      <c r="R5" s="64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="B6" s="65"/>
+      <c r="P6" s="96"/>
+      <c r="R6" s="96" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
0.1.3: requiredKt has accidentaly been missing from meta2xml.xml definition.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectKtAnnotationSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557774BA-60CE-F34C-9DF8-B6D4C6C393FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECCC0E-BE39-DD40-AFA2-C1434C1BE4B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9180" yWindow="2100" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,6 +1247,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1269,15 +1278,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1694,7 +1694,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1859,12 +1859,12 @@
         <v>2</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="88"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="91"/>
       <c r="G11" s="82"/>
       <c r="H11" s="69"/>
       <c r="I11" s="69"/>
@@ -2445,73 +2445,73 @@
       <c r="S37" s="15"/>
     </row>
     <row r="38" spans="1:19" ht="13.5" customHeight="1">
-      <c r="A38" s="90" t="s">
+      <c r="A38" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="B38" s="90" t="s">
+      <c r="B38" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="89" t="s">
+      <c r="C38" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="89" t="s">
+      <c r="D38" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="91" t="s">
+      <c r="E38" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="F38" s="89" t="s">
+      <c r="F38" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="91" t="s">
+      <c r="G38" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="91" t="s">
+      <c r="H38" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="I38" s="91" t="s">
+      <c r="I38" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="J38" s="94" t="s">
+      <c r="J38" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="K38" s="94" t="s">
+      <c r="K38" s="87" t="s">
         <v>83</v>
       </c>
-      <c r="L38" s="94" t="s">
+      <c r="L38" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="M38" s="94" t="s">
+      <c r="M38" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="N38" s="94" t="s">
+      <c r="N38" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="O38" s="89" t="s">
+      <c r="O38" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="P38" s="89"/>
+      <c r="P38" s="92"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="17"/>
       <c r="S38" s="9"/>
     </row>
     <row r="39" spans="1:19">
-      <c r="A39" s="90"/>
-      <c r="B39" s="90"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="92"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="95"/>
-      <c r="L39" s="95"/>
-      <c r="M39" s="95"/>
-      <c r="N39" s="95"/>
-      <c r="O39" s="89"/>
-      <c r="P39" s="89"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="95"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="88"/>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88"/>
+      <c r="M39" s="88"/>
+      <c r="N39" s="88"/>
+      <c r="O39" s="92"/>
+      <c r="P39" s="92"/>
       <c r="Q39" s="18"/>
       <c r="R39" s="30"/>
       <c r="S39" s="15"/>
@@ -2926,8 +2926,8 @@
     </row>
     <row r="6" spans="1:18">
       <c r="B6" s="65"/>
-      <c r="P6" s="96"/>
-      <c r="R6" s="96" t="s">
+      <c r="P6" s="86"/>
+      <c r="R6" s="86" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>